<commit_message>
sorted txt file and merge files
</commit_message>
<xml_diff>
--- a/config/Config.xlsx
+++ b/config/Config.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7010" tabRatio="481"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7010" tabRatio="481" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WiFi on-off" sheetId="1" r:id="rId1"/>
-    <sheet name="Logic Unit" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId3"/>
+    <sheet name="disconnect" sheetId="6" r:id="rId2"/>
+    <sheet name="Logic Unit" sheetId="7" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="193">
   <si>
     <t>TAG</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -31,12 +32,20 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>setWifiEnabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>client mode active</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>logs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">653770 07-01 10:13:19.510  1441  3783 I WifiService: setWifiEnabled package=com.android.settings uid=1000 </t>
+      <t xml:space="preserve">653227 07-01 11:26:11.815  1441  2008 I WifiService: setWifiEnabled package=com.android.settings uid=1000 </t>
     </r>
     <r>
       <rPr>
@@ -47,7 +56,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>enable=true</t>
+      <t>enable=false</t>
     </r>
     <r>
       <rPr>
@@ -63,10 +72,252 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">653770 07-01 10:13:19.510  1441  3783 I WifiService: setWifiEnabled package=com.android.settings uid=1000 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>enable=true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Note</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">110657 07-01 14:55:53.951  1441  2029 D WifiClientModeManager: STA iface wlan0 was destroyed, stopping client mode
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Next action:
+考虑交叉的场景
+110121 07-01 14:55:52.560  1441  6305 I WifiService: setWifiEnabled package=com.android.settings uid=1000 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>enable=false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+110152 07-01 14:55:52.568  1441  2028 D WifiController: WifiController.StaEnabledState: Turn WiFi OFF without any delay
+110595 07-01 14:55:53.607  1441  2187 I WifiService: setWifiEnabled package=com.android.settings uid=1000 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>enable=true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+110657 07-01 14:55:53.951  1441  2029 D WifiClientModeManager: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>STA iface wlan0 was destroyed, stopping client mode</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">connectToUserSelectNetwork </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07-01 14:04:00.589  1441  2029 D WifiStateMachine: connectToUserSelectNetwork netId 2, uid 1000, forceReconnect = false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User select network to connect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07-01 14:04:00.763 29003 29003 D wpa_supplicant: wlan0: State: DISCONNECTED -&gt; ASSOCIATING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:00.998 29003 29003 D wpa_supplicant: wlan0: State: ASSOCIATING -&gt; ASSOCIATED
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:01.012 29003 29003 D wpa_supplicant: wlan0: State: ASSOCIATED -&gt; 4WAY_HANDSHAKE
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:01.041 29003 29003 D wpa_supplicant: wlan0: State: 4WAY_HANDSHAKE -&gt; 4WAY_HANDSHAKE
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:01.046 29003 29003 D wpa_supplicant: wlan0: State: 4WAY_HANDSHAKE -&gt; GROUP_HANDSHAKE
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wlan0: State: 4WAY_HANDSHAKE -&gt; GROUP_HANDSHAKE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:01.059 29003 29003 D wpa_supplicant: wlan0: State: GROUP_HANDSHAKE -&gt; COMPLETED
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07-01 14:04:01.059 29003 29003 I wpa_supplicant: wlan0: CTRL-EVENT-CONNECTED - Connection to 18:31:bf:a8:ef:60 completed [id=0 id_str=%7B%22configKey%22%3A%22%5C%22WCG24%5C%22WPA_PSK%22%2C%22creatorUid%22%3A%221000%22%7D]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:03.224  1441 29014 D DhcpClient: Broadcasting DHCPDISCOVER
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wlan0: State: GROUP_HANDSHAKE -&gt; COMPLETED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GROUP_HANDSHAKE start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GROUP_HANDSHAKE done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Association start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Association done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4WAY_HANDSHAKE start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:03.550  1441 29014 D DhcpClient: Confirmed lease: IP address 192.168.50.113/24 Gateway 192.168.50.1  DNS servers: [ 192.168.50.1 ] Domains  DHCP server /192.168.50.1 Vendor info null lease 86400 seconds
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:03:57.829  1441  2029 I WifiStateMachine: Connecting with 60:1d:91:57:fc:b1 as the mac address
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>as the mac address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DHCP discover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DHCP offer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:03.514  1441 29108 D DhcpClient: Received packet: 60:1d:91:57:fc:b1 OFFER, ip /192.168.50.113, mask /255.255.255.0, DNS servers: /192.168.50.1 , gateways [/192.168.50.1] lease time 86400, domain null
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:03.520  1441 29014 D DhcpClient: Broadcasting DHCPREQUEST ciaddr=0.0.0.0 request=192.168.50.113 serverid=192.168.50.1
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DHCP request</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:03.548  1441 29108 D DhcpClient: Received packet: 60:1d:91:57:fc:b1 ACK: your new IP /192.168.50.113, netmask /255.255.255.0, gateways [/192.168.50.1] DNS servers: /192.168.50.1 , lease time 86400
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DHCP ACK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Confirmed lease: IP address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:03.632  1441  2029 D WifiStateMachine: setDetailed state, old =OBTAINING_IPADDR and new state=CONNECTED hidden=false isLFRDHCPRenewRequired=false
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wlan0: State: ASSOCIATING -&gt; ASSOCIATED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07-01 14:04:00.757 29003 29003 I wpa_supplicant: wlan0: Trying to associate with SSID 'WCG24'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">07-01 14:04:00.624  1441  2029 D SupplicantStaIfaceHal: connectToNetwork "WCG24"WPA_PSK
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Logic ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -87,6 +338,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>OUTPUT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>KEYWORD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,6 +350,54 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Turn on WiFi failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turned on WiFi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turning off WiFi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turned off WiFi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turn off WiFi failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">654680 07-01 10:13:21.829  1441  2029 D WifiStateMachinePrime: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client mode active</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>("enable=“,  )</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -107,6 +410,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">CTRL-EVENT-CONNECTED - Connection to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;VAL1&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> completed</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>OUTPUT2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -119,7 +450,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>KEYWORD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STA iface wlan0 was destroyed, stopping client mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2 (KEYWORD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+L1 (VAL1,false)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAL2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUT2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>VALUE_FLAG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MANDATORY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -136,11 +496,182 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>L2 (KEYWORD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2 (KEYWORD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(“Connecting with”， “as the mac address”）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">connectToNetwork </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>DUT-MAC=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;VAL1&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">connectToNetwork </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;VAL1&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trying to associate with SSID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>("Trying to associate with SSID", )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>("connectToNetwork", )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trying to associate with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;VAL1&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wlan0: State: DISCONNECTED -&gt; ASSOCIATING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4WAY_HANDSHAKE done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>KEYWORD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>open网络没有四次握手和组密钥交换过程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2 (KEYWORD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL-EVENT-CONNECTED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DhcpClient: Broadcasting DHCPDISCOVER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>wifi_on_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_on_2</t>
+  </si>
+  <si>
+    <t>wifi_off_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_off_2</t>
+  </si>
+  <si>
+    <t>wifi_connected_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_connected_5</t>
+  </si>
+  <si>
+    <t>wifi_connected_6</t>
+  </si>
+  <si>
+    <t>wifi_connected_7</t>
+  </si>
+  <si>
+    <t>wifi_connected_8</t>
+  </si>
+  <si>
+    <t>wifi_connected_9</t>
+  </si>
+  <si>
+    <t>wifi_connected_10</t>
+  </si>
+  <si>
+    <t>wifi_connected_12</t>
+  </si>
+  <si>
+    <t>wifi_connected_13</t>
+  </si>
+  <si>
+    <t>wifi_connected_14</t>
+  </si>
+  <si>
+    <t>wifi_connected_15</t>
+  </si>
+  <si>
+    <t>wifi_connected_16</t>
+  </si>
+  <si>
+    <t>wifi_connected_17</t>
+  </si>
+  <si>
+    <t>wifi_connected_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connection to &lt;wifi_connected_4.VAL1&gt; failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4WAY_HANDSHAKE failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>("Connection to", "completed")</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -178,7 +709,143 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>OFFER, ip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2 (KEYWORD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DhcpClient: Broadcasting DHCPREQUEST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACK: your new IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>("IP address", "Gateway")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>("Gateway", "DNS servers")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_connected_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_connected_11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_connected_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WiFi Connected to AP </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;wifi_connected_3.VAL1&gt;, with BSSID: &lt;wifi_connected_11.VAL1&gt;, IP: &lt;wifi_connected_16.VAL1&gt;, DUT mac: &lt;wifi_connected_2.VAL1&gt; </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Obtained IP address: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;VAL1&gt;, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gateway:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;VAL2&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_disconnect_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_disconnect_2</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_3</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_4</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_5</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_6</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_7</t>
+  </si>
+  <si>
+    <t>FORGET_NETWORK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>old =OBTAINING_IPADDR and new state=CONNECTED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User forget network</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>L3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">151171 07-04 15:30:43.574  1789  2271 D WifiStateMachine:  ConnectedState !FORGET_NETWORK uid=1000 rt=131457/131457 0 0
+151172 07-04 15:30:43.574  1789  2271 D WifiStateMachine:  L2ConnectedState !FORGET_NETWORK uid=1000 rt=131457/131457 0 0
+151173 07-04 15:30:43.574  1789  2271 D WifiStateMachine:  ConnectModeState !FORGET_NETWORK uid=1000 rt=131458/131458 0 0
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -187,7 +854,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">07-04 00:05:20.386 13334 13334 I wpa_supplicant: wlan0: CTRL-EVENT-DISCONNECTED bssid=18:31:bf:a8:ef:60 reason=3 locally_generated=1 disconnect_rssi=0
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（“bssid=“， ”reason”）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> （"reason=", "locally_generated"）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>("locally_generated=",  "disconnect_rssi")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAL4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>("disconnect_rssi=", )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>(VAL1, STRING)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL-EVENT-DISCONNECTED</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -265,6 +961,149 @@
  </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL-EVENT-ASSOC-REJECT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>("bssid=", )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CTRL-EVENT-ASSOC-REJECT bssid=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;VAL1&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L3 (KEYWORD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L4 (KEYWORD, 3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HB missed from AP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2 (KEYWORD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heartbeat Failure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IpReachabilityMonitor: FAILURE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IPR Failure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wma_peer_sta_kickout_event_handler: PEER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>("PEER:[", "], ADDR")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Station is kicked out by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;VAL1&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eSIR_MAC_CLASS2_FRAME_FROM_NON_AUTH_STA_REASON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_disconnect_8</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_9</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_10</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_11</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_12</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_13</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_14</t>
+  </si>
+  <si>
+    <t>wifi_disconnect_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eSIR_MAC_UNSPEC_FAILURE_REASON </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eSIR_MAC_PREV_AUTH_NOT_VALID_REASON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eSIR_MAC_DEAUTH_LEAVING_BSS_REASON </t>
+  </si>
+  <si>
+    <t>eSIR_MAC_DISASSOC_DUE_TO_INACTIVITY_REASON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eSIR_MAC_DISASSOC_DUE_TO_DISABILITY_REASON </t>
+  </si>
+  <si>
+    <t xml:space="preserve">eSIR_MAC_CLASS2_FRAME_FROM_NON_AUTH_STA_REASON </t>
+  </si>
+  <si>
+    <t xml:space="preserve">eSIR_MAC_CLASS3_FRAME_FROM_NON_ASSOC_STA_REASON </t>
+  </si>
+  <si>
+    <t xml:space="preserve">eSIR_MAC_DISASSOC_LEAVING_BSS_REASON </t>
+  </si>
+  <si>
+    <t>eSIR_MAC_4WAY_HANDSHAKE_TIMEOUT_REASON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eSIR_MAC_STA_NOT_PRE_AUTHENTICATED_REASON </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi_disconnect_20</t>
   </si>
   <si>
     <t xml:space="preserve">wifi连接过程中可能遇到的错误/失败：
@@ -750,6 +1589,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>07-01 14:04:00.862 29003 29003 wpa_supplicant: wlan0: CTRL-EVENT-ASSOC-REJECT bssid=a0:ab:1b:e6:c9:eb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wlan0: State: 4WAY_HANDSHAKE -&gt; 4WAY_HANDSHAKE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wlan0: State: ASSOCIATED -&gt; 4WAY_HANDSHAKE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">有些流程可能不会出现，比如四次握手和DHCP，但是一旦出现该流程，就必须成功执行，否则该过程失败:
 </t>
@@ -851,15 +1702,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LEVEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>setWifiEnabled</t>
+    <t xml:space="preserve">setWifiEnabled </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -867,7 +1710,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -911,6 +1754,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -982,7 +1833,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1018,11 +1869,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1047,10 +1918,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1070,8 +1947,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1125,34 +2011,67 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1435,543 +2354,539 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16.4140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="42.83203125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.08203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="22.58203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="17.58203125" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
-    <col min="9" max="9" width="33.58203125" customWidth="1"/>
-    <col min="10" max="11" width="28.33203125" customWidth="1"/>
-    <col min="12" max="12" width="101.33203125" style="9" customWidth="1"/>
-    <col min="13" max="13" width="127.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.4140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.08203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="22.58203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="30" customWidth="1"/>
+    <col min="6" max="6" width="17.58203125" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="33.58203125" customWidth="1"/>
+    <col min="9" max="10" width="28.33203125" customWidth="1"/>
+    <col min="11" max="11" width="101.33203125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="127.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="15.5">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="40" t="s">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="57" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="26">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="57" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="59">
+        <v>1</v>
+      </c>
+      <c r="D3" s="60">
+        <v>0</v>
+      </c>
+      <c r="E3" s="61"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="11" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="48" customFormat="1" ht="76" customHeight="1">
-      <c r="A2" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="21">
+      <c r="C4" s="26">
         <v>1</v>
       </c>
-      <c r="E2" s="11">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="F2" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="35" customFormat="1" ht="76" customHeight="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="L3" s="36"/>
-    </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="76" customHeight="1">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="36"/>
-    </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="76" customHeight="1">
-      <c r="C5" s="36"/>
-      <c r="D5" s="38"/>
-      <c r="F5" s="39"/>
-      <c r="L5" s="36"/>
-    </row>
-    <row r="6" spans="1:13" ht="76" customHeight="1">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="E6"/>
-    </row>
-    <row r="7" spans="1:13" ht="39" customHeight="1">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="E7"/>
-    </row>
-    <row r="8" spans="1:13" ht="39" customHeight="1">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="E8"/>
-    </row>
-    <row r="9" spans="1:13" s="1" customFormat="1">
+      <c r="E4" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="11" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="26">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="63"/>
+      <c r="H5" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="40" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="K6" s="41"/>
+    </row>
+    <row r="7" spans="1:12" s="40" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="41"/>
+    </row>
+    <row r="8" spans="1:12" s="40" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="41"/>
+      <c r="C8" s="43"/>
+      <c r="E8" s="44"/>
+      <c r="K8" s="41"/>
+    </row>
+    <row r="9" spans="1:12" ht="76" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="12"/>
-      <c r="E9"/>
-      <c r="F9" s="25"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="E10"/>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="E11"/>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12"/>
-      <c r="B12"/>
-      <c r="E12"/>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="B12" s="9"/>
+      <c r="C12" s="14"/>
+      <c r="D12"/>
+      <c r="E12" s="30"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13"/>
-      <c r="B13"/>
-      <c r="E13"/>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="E14"/>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15"/>
-      <c r="B15"/>
-      <c r="E15"/>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="E16"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="D16"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="E17"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="D17"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="E18"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="D18"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19"/>
-      <c r="B19"/>
-      <c r="E19"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="D19"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20"/>
-      <c r="B20"/>
-      <c r="E20"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="D20"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21"/>
-      <c r="B21"/>
-      <c r="E21"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22"/>
-      <c r="B22"/>
-      <c r="E22"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="D22"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23"/>
-      <c r="B23"/>
-      <c r="E23"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="D23"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24"/>
-      <c r="B24"/>
-      <c r="E24"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25"/>
-      <c r="B25"/>
-      <c r="E25"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="D25"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26"/>
-      <c r="B26"/>
-      <c r="E26"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27"/>
-      <c r="B27"/>
-      <c r="E27"/>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28"/>
-      <c r="B28"/>
-      <c r="E28"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29"/>
-      <c r="B29"/>
-      <c r="E29"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30"/>
-      <c r="B30"/>
-      <c r="E30"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31"/>
-      <c r="B31"/>
-      <c r="E31"/>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32"/>
-      <c r="B32"/>
-      <c r="E32"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33"/>
-      <c r="B33"/>
-      <c r="E33"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34"/>
-      <c r="B34"/>
-      <c r="E34"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35"/>
-      <c r="B35"/>
-      <c r="E35"/>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36"/>
-      <c r="B36"/>
-      <c r="E36"/>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37"/>
-      <c r="B37"/>
-      <c r="E37"/>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38"/>
-      <c r="B38"/>
-      <c r="E38"/>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39"/>
-      <c r="B39"/>
-      <c r="E39"/>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40"/>
-      <c r="B40"/>
-      <c r="E40"/>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41"/>
-      <c r="B41"/>
-      <c r="E41"/>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42"/>
-      <c r="B42"/>
-      <c r="E42"/>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43"/>
-      <c r="B43"/>
-      <c r="E43"/>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44"/>
-      <c r="B44"/>
-      <c r="E44"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45"/>
-      <c r="B45"/>
-      <c r="E45"/>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46"/>
-      <c r="B46"/>
-      <c r="E46"/>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47"/>
-      <c r="B47"/>
-      <c r="E47"/>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48"/>
-      <c r="B48"/>
-      <c r="E48"/>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="D48"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49"/>
-      <c r="B49"/>
-      <c r="E49"/>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="D49"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50"/>
-      <c r="B50"/>
-      <c r="E50"/>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="D50"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51"/>
-      <c r="B51"/>
-      <c r="E51"/>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="D51"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52"/>
-      <c r="B52"/>
-      <c r="E52"/>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="D52"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53"/>
-      <c r="B53"/>
-      <c r="E53"/>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="D53"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54"/>
-      <c r="B54"/>
-      <c r="E54"/>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="D54"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55"/>
-      <c r="B55"/>
-      <c r="E55"/>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="D55"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56"/>
-      <c r="B56"/>
-      <c r="E56"/>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="D56"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57"/>
-      <c r="B57"/>
-      <c r="E57"/>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="D57"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58"/>
-      <c r="B58"/>
-      <c r="E58"/>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="D58"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59"/>
-      <c r="B59"/>
-      <c r="E59"/>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="D59"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60"/>
-      <c r="B60"/>
-      <c r="E60"/>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="D60"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61"/>
-      <c r="B61"/>
-      <c r="E61"/>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="D61"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62"/>
-      <c r="B62"/>
-      <c r="E62"/>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="D62"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63"/>
-      <c r="B63"/>
-      <c r="E63"/>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="D63"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64"/>
-      <c r="B64"/>
-      <c r="E64"/>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="D64"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65"/>
-      <c r="B65"/>
-      <c r="E65"/>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="D65"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66"/>
-      <c r="B66"/>
-      <c r="E66"/>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="D66"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67"/>
-      <c r="B67"/>
-      <c r="E67"/>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="D67"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68"/>
-      <c r="B68"/>
-      <c r="E68"/>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="D68"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69"/>
-      <c r="B69"/>
-      <c r="E69"/>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="D69"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70"/>
-      <c r="B70"/>
-      <c r="E70"/>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="D70"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71"/>
-      <c r="B71"/>
-      <c r="E71"/>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="D71"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72"/>
-      <c r="B72"/>
-      <c r="E72"/>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="D72"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73"/>
-      <c r="B73"/>
-      <c r="E73"/>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="D73"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74"/>
-      <c r="B74"/>
-      <c r="E74"/>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="D74"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75"/>
-      <c r="B75"/>
-      <c r="E75"/>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="D75"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76"/>
-      <c r="B76"/>
-      <c r="E76"/>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="D76"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77"/>
-      <c r="B77"/>
-      <c r="E77"/>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="D77"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78"/>
-      <c r="B78"/>
-      <c r="E78"/>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="D78"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79"/>
-      <c r="B79"/>
-      <c r="E79"/>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="D79"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80"/>
-      <c r="B80"/>
-      <c r="E80"/>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="D80"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81"/>
-      <c r="B81"/>
-      <c r="E81"/>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="D81"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82"/>
-      <c r="B82"/>
-      <c r="E82"/>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="D82"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83"/>
-      <c r="B83"/>
-      <c r="E83"/>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="D83"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84"/>
-      <c r="B84"/>
-      <c r="E84"/>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="D84"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85"/>
-      <c r="B85"/>
-      <c r="E85"/>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="D85"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86"/>
-      <c r="B86"/>
-      <c r="E86"/>
+      <c r="D86"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87"/>
+      <c r="D87"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88"/>
+      <c r="D88"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89"/>
+      <c r="D89"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1982,177 +2897,1022 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.4140625" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="39" style="29" customWidth="1"/>
-    <col min="4" max="4" width="138.5" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="53.25" customWidth="1"/>
+    <col min="3" max="3" width="31.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36" style="9" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="8" width="34.9140625" customWidth="1"/>
+    <col min="9" max="9" width="38" style="9" customWidth="1"/>
+    <col min="10" max="10" width="133.6640625" customWidth="1"/>
+    <col min="11" max="11" width="58.58203125" customWidth="1"/>
+    <col min="12" max="12" width="112.4140625" customWidth="1"/>
+    <col min="13" max="13" width="64.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="8" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="69" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="66" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="26">
+        <v>0</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="26">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="26">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="26">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="15"/>
+      <c r="L5" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="26">
+        <v>0</v>
+      </c>
+      <c r="D6" s="26">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="26">
+        <v>0</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0</v>
+      </c>
+      <c r="D8" s="26">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="15"/>
+      <c r="L8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0</v>
+      </c>
+      <c r="D9" s="26">
+        <v>0</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="K9" s="15"/>
+      <c r="L9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="26">
+        <v>0</v>
+      </c>
+      <c r="D10" s="26">
+        <v>0</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="26">
+        <v>0</v>
+      </c>
+      <c r="D11" s="26">
+        <v>0</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="15"/>
+      <c r="L11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="26">
+        <v>0</v>
+      </c>
+      <c r="D12" s="26">
+        <v>0</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="15"/>
+      <c r="L12" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="26">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="21"/>
+    </row>
+    <row r="14" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="26">
+        <v>0</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="26">
+        <v>0</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" ht="66" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="27" t="s">
+    </row>
+    <row r="16" spans="1:13" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="26">
+        <v>0</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="83" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="179" customHeight="1">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="17" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="26">
+        <v>0</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="26">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="45" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="42"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
-    </row>
-    <row r="7" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="3"/>
+    </row>
+    <row r="19" spans="1:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="A19" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="67">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="56" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="6">
+        <v>1</v>
+      </c>
+      <c r="D35" s="6">
+        <v>4</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2163,31 +3923,212 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.4140625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="39" style="34" customWidth="1"/>
+    <col min="4" max="4" width="138.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="83" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="179" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="53" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="52"/>
+    </row>
+    <row r="7" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="78.08203125" customWidth="1"/>
     <col min="2" max="2" width="45.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="110.5" customHeight="1">
+    <row r="1" spans="1:1" ht="110.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="106.5" customHeight="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="130.5" customHeight="1">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>37</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Modified the content of volume "MANDATORY" 2. Update the "Comment" sheet.
</commit_message>
<xml_diff>
--- a/config/Config.xlsx
+++ b/config/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7010" tabRatio="737" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7010" tabRatio="737" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Parse-P" sheetId="11" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="WiFi on-off_P" sheetId="1" r:id="rId3"/>
     <sheet name="WiFi connect-disconnect_P" sheetId="6" r:id="rId4"/>
     <sheet name="Logic Unit" sheetId="7" r:id="rId5"/>
-    <sheet name="Comment" sheetId="8" r:id="rId6"/>
+    <sheet name="Comment" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="236">
   <si>
     <t>TAG</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -564,40 +564,6 @@
   </si>
   <si>
     <t>4WAY_HANDSHAKE failed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>有些关键字不是唯一的，但是后面跟的内容是不一样的，这样同时可以确定：
-DhcpClient: Received packet: 60:1d:91:57:fc:b1 OFFER, ip
-DhcpClient: Received packet: 60:1d:91:57:fc:b1 ACK: your new IP
-别的模块也有可能遇到这种情况，
-1. 根据[</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不确定因素</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]后面的内容才能唯一确定关键字
-2. 每一行的关键字一样，具体的内容不同，可以使用逻辑1
-3. 一行里面有很多的不确定因素需要提取</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1411,107 +1377,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">有些流程可能不会出现，比如四次握手和DHCP，但是一旦出现该流程，就必须成功执行，否则该过程失败:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1. 四次握手过程：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1.1 可以重复，重复收到1/4或者3/4的消息不算error; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>error的log是什么？</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1.2 但一旦出现失败的消息，return;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2. DHCP过程类似：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.1 可以重复，重复发送DHCP DISCOVER不算失败，可以重复；</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">最多可以重复几次
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2.2 一旦出现失败log，return</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">404796 07-16 17:14:18.070  8646  8646 I wpa_supplicant: wlan0: CTRL-EVENT-CONNECTED - Connection to 18:31:bf:a8:ef:60 completed [id=0 id_str=%7B%22configKey%22%3A%22%5C%22WCG24%5C%22WPA_PSK%22%2C%22creatorUid%22%3A%221000%22%7D]
 405746 07-16 17:14:29.375  1658  2269 D WifiStateMachine: connectToUserSelectNetwork netId 5, uid 1000, forceReconnect = true
 405754 07-16 17:14:29.436  8646  8646 I wpa_supplicant: wlan0: CTRL-EVENT-DISCONNECTED bssid=18:31:bf:a8:ef:60 reason=3 locally_generated=1 disconnect_rssi=47
@@ -1594,14 +1459,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>WiFi on-off_P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WiFi connect-disconnect_P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Function</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1795,6 +1652,279 @@
   </si>
   <si>
     <t>bssid=,#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">11299
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sub Module
+(1: STA; 2: SoftAp; 3: P2P; ...)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subprocess
+(wifi on step 1, wifi on step2...)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi disconnect
+(11300 ~ 11399)
+11399表示wifi connect结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5-9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reserved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SoftAp connect
+( 12200 - 12299)
+12299表示softAp off结束
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SoftAp disconnect
+( 12300 - 12399)
+12199表示softAp off结束
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P2P on 
+( 13000 - 13099)
+13099表示P2P on结束
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P2P off 
+( 13100 - 13199)
+13199表示P2P off结束
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P2P Invite + GO negotiation
+( 13200 - 13299)
+13299表示P2P GO negotiation结束
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P2P connect 
+( 13300 - 13399)
+13399表示P2P connect结束
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P2P disconnect
+( 13400 - 13499)
+13499表示P2P disconnect结束
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Module
+[1: WiFi; 2: BT; 3: LBS; 4: NFC; ...]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi connect
+(11200 ~ 11299)
+11299表示wifi connect结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi scan
+(11400 ~ 11499)
+11499表示wifi scan结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5-9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SoftAp on
+(12000 - 12099)
+12099表示softAp on结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SoftAp off
+( 12100 - 12199)
+12199表示softAp off结束
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Process
+(0: wifi on; 1: wifi off; 2: wifi connect; 
+3: wifi disconnect; 4: wifi scan...)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi on
+(11000 ~11099)
+11099表示wifi on过程结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wifi off
+(11100~11199)
+11199表示wifi off结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>有些关键字不是唯一的，但是后面跟的内容是不一样的，这样同时可以确定：
+DhcpClient: Received packet: 60:1d:91:57:fc:b1 OFFER, ip
+DhcpClient: Received packet: 60:1d:91:57:fc:b1 ACK: your new IP
+别的模块也有可能遇到这种情况，
+1. 根据[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不确定因素</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]后面的内容才能唯一确定关键字
+2. 每一行的关键字一样，具体的内容不同，可以使用逻辑1
+3. 一行里面有很多的不确定因素需要提取</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">有些流程可能不会出现，比如四次握手和DHCP，但是一旦出现该流程，就必须成功执行，否则该过程失败:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1. 四次握手过程：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1.1 可以重复，重复收到1/4或者3/4的消息不算error; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>error的log是什么？</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1.2 但一旦出现失败的消息，return;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. DHCP过程类似：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.1 可以重复，重复发送DHCP DISCOVER不算失败，可以重复；</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">最多可以重复几次
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.2 一旦出现失败log，return</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1802,7 +1932,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1892,6 +2022,39 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="3"/>
@@ -1899,7 +2062,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1927,6 +2090,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1991,7 +2178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2197,6 +2384,67 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2483,66 +2731,66 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="70" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2560,66 +2808,66 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="13.25" customWidth="1"/>
     <col min="2" max="2" width="23.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="70" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2633,11 +2881,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="16.4140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="16.4140625" style="77" customWidth="1"/>
@@ -2653,18 +2901,18 @@
     <col min="13" max="13" width="127.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="15.5">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>64</v>
@@ -2694,50 +2942,50 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="57" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="57" customFormat="1" ht="76" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>81</v>
       </c>
       <c r="B2" s="72" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>55</v>
       </c>
       <c r="D2" s="26">
-        <v>1</v>
+        <v>11000</v>
       </c>
       <c r="E2" s="12">
         <v>1</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="57" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="57" customFormat="1" ht="76" customHeight="1">
       <c r="A3" s="55" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="73" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C3" s="58" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="59">
-        <v>1</v>
+        <v>11099</v>
       </c>
       <c r="E3" s="60">
         <v>0</v>
@@ -2758,24 +3006,24 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="11" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="11" customFormat="1" ht="76" customHeight="1">
       <c r="A4" s="55" t="s">
         <v>83</v>
       </c>
       <c r="B4" s="72" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="26">
-        <v>1</v>
+        <v>11100</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>61</v>
@@ -2787,18 +3035,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="11" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="11" customFormat="1" ht="73.5" customHeight="1">
       <c r="A5" s="55" t="s">
         <v>84</v>
       </c>
       <c r="B5" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="26">
-        <v>1</v>
+        <v>11199</v>
       </c>
       <c r="E5" s="12">
         <v>0</v>
@@ -2817,10 +3065,10 @@
         <v>8</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1">
       <c r="A6" s="35"/>
       <c r="B6" s="74"/>
       <c r="C6" s="36"/>
@@ -2831,7 +3079,7 @@
       <c r="H6" s="16"/>
       <c r="L6" s="41"/>
     </row>
-    <row r="7" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1">
       <c r="A7" s="35"/>
       <c r="B7" s="74"/>
       <c r="C7" s="36"/>
@@ -2844,29 +3092,29 @@
       <c r="K7" s="42"/>
       <c r="L7" s="41"/>
     </row>
-    <row r="8" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1">
       <c r="B8" s="75"/>
       <c r="C8" s="41"/>
       <c r="D8" s="43"/>
       <c r="F8" s="44"/>
       <c r="L8" s="41"/>
     </row>
-    <row r="9" spans="1:13" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="76" customHeight="1">
       <c r="A9"/>
       <c r="B9" s="76"/>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="39" customHeight="1">
       <c r="A10"/>
       <c r="B10" s="76"/>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="39" customHeight="1">
       <c r="A11"/>
       <c r="B11" s="76"/>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="1" customFormat="1">
       <c r="A12"/>
       <c r="B12" s="76"/>
       <c r="C12" s="9"/>
@@ -2880,387 +3128,387 @@
       <c r="K12"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13"/>
       <c r="B13" s="76"/>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14"/>
       <c r="B14" s="76"/>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15"/>
       <c r="B15" s="76"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16"/>
       <c r="B16" s="76"/>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17"/>
       <c r="B17" s="76"/>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18"/>
       <c r="B18" s="76"/>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19"/>
       <c r="B19" s="76"/>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20"/>
       <c r="B20" s="76"/>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21"/>
       <c r="B21" s="76"/>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22"/>
       <c r="B22" s="76"/>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23"/>
       <c r="B23" s="76"/>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24"/>
       <c r="B24" s="76"/>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25"/>
       <c r="B25" s="76"/>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26"/>
       <c r="B26" s="76"/>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27"/>
       <c r="B27" s="76"/>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28"/>
       <c r="B28" s="76"/>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29"/>
       <c r="B29" s="76"/>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5">
       <c r="A30"/>
       <c r="B30" s="76"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5">
       <c r="A31"/>
       <c r="B31" s="76"/>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5">
       <c r="A32"/>
       <c r="B32" s="76"/>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5">
       <c r="A33"/>
       <c r="B33" s="76"/>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5">
       <c r="A34"/>
       <c r="B34" s="76"/>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35"/>
       <c r="B35" s="76"/>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36"/>
       <c r="B36" s="76"/>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37"/>
       <c r="B37" s="76"/>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5">
       <c r="A38"/>
       <c r="B38" s="76"/>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5">
       <c r="A39"/>
       <c r="B39" s="76"/>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40"/>
       <c r="B40" s="76"/>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5">
       <c r="A41"/>
       <c r="B41" s="76"/>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5">
       <c r="A42"/>
       <c r="B42" s="76"/>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5">
       <c r="A43"/>
       <c r="B43" s="76"/>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5">
       <c r="A44"/>
       <c r="B44" s="76"/>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5">
       <c r="A45"/>
       <c r="B45" s="76"/>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5">
       <c r="A46"/>
       <c r="B46" s="76"/>
       <c r="E46"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5">
       <c r="A47"/>
       <c r="B47" s="76"/>
       <c r="E47"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5">
       <c r="A48"/>
       <c r="B48" s="76"/>
       <c r="E48"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5">
       <c r="A49"/>
       <c r="B49" s="76"/>
       <c r="E49"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5">
       <c r="A50"/>
       <c r="B50" s="76"/>
       <c r="E50"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5">
       <c r="A51"/>
       <c r="B51" s="76"/>
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5">
       <c r="A52"/>
       <c r="B52" s="76"/>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5">
       <c r="A53"/>
       <c r="B53" s="76"/>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5">
       <c r="A54"/>
       <c r="B54" s="76"/>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5">
       <c r="A55"/>
       <c r="B55" s="76"/>
       <c r="E55"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5">
       <c r="A56"/>
       <c r="B56" s="76"/>
       <c r="E56"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5">
       <c r="A57"/>
       <c r="B57" s="76"/>
       <c r="E57"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5">
       <c r="A58"/>
       <c r="B58" s="76"/>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5">
       <c r="A59"/>
       <c r="B59" s="76"/>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5">
       <c r="A60"/>
       <c r="B60" s="76"/>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5">
       <c r="A61"/>
       <c r="B61" s="76"/>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5">
       <c r="A62"/>
       <c r="B62" s="76"/>
       <c r="E62"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5">
       <c r="A63"/>
       <c r="B63" s="76"/>
       <c r="E63"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5">
       <c r="A64"/>
       <c r="B64" s="76"/>
       <c r="E64"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5">
       <c r="A65"/>
       <c r="B65" s="76"/>
       <c r="E65"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5">
       <c r="A66"/>
       <c r="B66" s="76"/>
       <c r="E66"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5">
       <c r="A67"/>
       <c r="B67" s="76"/>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5">
       <c r="A68"/>
       <c r="B68" s="76"/>
       <c r="E68"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5">
       <c r="A69"/>
       <c r="B69" s="76"/>
       <c r="E69"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5">
       <c r="A70"/>
       <c r="B70" s="76"/>
       <c r="E70"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5">
       <c r="A71"/>
       <c r="B71" s="76"/>
       <c r="E71"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5">
       <c r="A72"/>
       <c r="B72" s="76"/>
       <c r="E72"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5">
       <c r="A73"/>
       <c r="B73" s="76"/>
       <c r="E73"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5">
       <c r="A74"/>
       <c r="B74" s="76"/>
       <c r="E74"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5">
       <c r="A75"/>
       <c r="B75" s="76"/>
       <c r="E75"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5">
       <c r="A76"/>
       <c r="B76" s="76"/>
       <c r="E76"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5">
       <c r="A77"/>
       <c r="B77" s="76"/>
       <c r="E77"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5">
       <c r="A78"/>
       <c r="B78" s="76"/>
       <c r="E78"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5">
       <c r="A79"/>
       <c r="B79" s="76"/>
       <c r="E79"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5">
       <c r="A80"/>
       <c r="B80" s="76"/>
       <c r="E80"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5">
       <c r="A81"/>
       <c r="B81" s="76"/>
       <c r="E81"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5">
       <c r="A82"/>
       <c r="B82" s="76"/>
       <c r="E82"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5">
       <c r="A83"/>
       <c r="B83" s="76"/>
       <c r="E83"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5">
       <c r="A84"/>
       <c r="B84" s="76"/>
       <c r="E84"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5">
       <c r="A85"/>
       <c r="B85" s="76"/>
       <c r="E85"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5">
       <c r="A86"/>
       <c r="B86" s="76"/>
       <c r="E86"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5">
       <c r="A87"/>
       <c r="B87" s="76"/>
       <c r="E87"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5">
       <c r="A88"/>
       <c r="B88" s="76"/>
       <c r="E88"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5">
       <c r="A89"/>
       <c r="B89" s="76"/>
       <c r="E89"/>
@@ -3276,11 +3524,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="21" style="78" customWidth="1"/>
@@ -3297,12 +3545,12 @@
     <col min="14" max="14" width="64.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="15.5">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>46</v>
@@ -3323,7 +3571,7 @@
         <v>56</v>
       </c>
       <c r="I1" s="69" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J1" s="24" t="s">
         <v>66</v>
@@ -3341,18 +3589,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="34.5" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D2" s="26">
-        <v>0</v>
+        <v>11200</v>
       </c>
       <c r="E2" s="12">
         <v>0</v>
@@ -3362,7 +3610,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>10</v>
@@ -3372,24 +3620,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="34.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="72" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="26">
-        <v>1</v>
+        <v>11201</v>
       </c>
       <c r="E3" s="12">
         <v>1</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -3405,24 +3653,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="39" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>98</v>
       </c>
       <c r="B4" s="72" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="26">
-        <v>1</v>
+        <v>11202</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -3435,27 +3683,27 @@
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="36" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="72" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D5" s="26">
-        <v>1</v>
+        <v>11203</v>
       </c>
       <c r="E5" s="12">
         <v>1</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -3471,18 +3719,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="24" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>86</v>
       </c>
       <c r="B6" s="72" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="26">
-        <v>0</v>
+        <v>11204</v>
       </c>
       <c r="E6" s="26">
         <v>0</v>
@@ -3492,7 +3740,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>23</v>
@@ -3502,51 +3750,51 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="24" customHeight="1">
       <c r="A7" s="65" t="s">
         <v>87</v>
       </c>
       <c r="B7" s="72" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="26">
-        <v>0</v>
+        <v>11205</v>
       </c>
       <c r="E7" s="26">
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L7" s="15"/>
       <c r="M7" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="25.5" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B8" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="26">
-        <v>0</v>
+        <v>11206</v>
       </c>
       <c r="E8" s="26">
         <v>0</v>
@@ -3566,18 +3814,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="25.5" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B9" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D9" s="26">
-        <v>0</v>
+        <v>11207</v>
       </c>
       <c r="E9" s="26">
         <v>0</v>
@@ -3600,18 +3848,18 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="25.5" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>89</v>
       </c>
       <c r="B10" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" s="26">
-        <v>0</v>
+        <v>11208</v>
       </c>
       <c r="E10" s="26">
         <v>0</v>
@@ -3633,18 +3881,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="25.5" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B11" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="26">
-        <v>0</v>
+        <v>11209</v>
       </c>
       <c r="E11" s="26">
         <v>0</v>
@@ -3664,18 +3912,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="25.5" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B12" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="26">
-        <v>0</v>
+        <v>11210</v>
       </c>
       <c r="E12" s="26">
         <v>0</v>
@@ -3695,24 +3943,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="25.5" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="72" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C13" s="49" t="s">
         <v>79</v>
       </c>
       <c r="D13" s="26">
-        <v>1</v>
+        <v>11211</v>
       </c>
       <c r="E13" s="12">
         <v>1</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -3731,18 +3979,18 @@
       </c>
       <c r="N13" s="21"/>
     </row>
-    <row r="14" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="29" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B14" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>80</v>
       </c>
       <c r="D14" s="26">
-        <v>0</v>
+        <v>11212</v>
       </c>
       <c r="E14" s="12">
         <v>0</v>
@@ -3762,18 +4010,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="46" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>93</v>
       </c>
       <c r="B15" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" s="26">
-        <v>0</v>
+        <v>11213</v>
       </c>
       <c r="E15" s="12">
         <v>0</v>
@@ -3783,7 +4031,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>30</v>
@@ -3793,18 +4041,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="46" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>94</v>
       </c>
       <c r="B16" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" s="26">
-        <v>0</v>
+        <v>11214</v>
       </c>
       <c r="E16" s="12">
         <v>0</v>
@@ -3814,7 +4062,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>33</v>
@@ -3824,18 +4072,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="46" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B17" s="72" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D17" s="26">
-        <v>0</v>
+        <v>11215</v>
       </c>
       <c r="E17" s="12">
         <v>0</v>
@@ -3845,7 +4093,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>35</v>
@@ -3855,53 +4103,53 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="42">
       <c r="A18" s="10" t="s">
         <v>96</v>
       </c>
       <c r="B18" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="26">
-        <v>0</v>
+        <v>11216</v>
       </c>
       <c r="E18" s="6">
         <v>1</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="42">
       <c r="A19" s="65" t="s">
         <v>97</v>
       </c>
       <c r="B19" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C19" s="66" t="s">
-        <v>119</v>
-      </c>
-      <c r="D19" s="67">
-        <v>1</v>
+        <v>118</v>
+      </c>
+      <c r="D19" s="67" t="s">
+        <v>211</v>
       </c>
       <c r="E19" s="6">
         <v>0</v>
@@ -3911,28 +4159,28 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="56" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="56">
       <c r="A20" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D20" s="6">
-        <v>0</v>
+        <v>11200</v>
       </c>
       <c r="E20" s="12">
         <v>0</v>
@@ -3942,26 +4190,26 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D21" s="6">
-        <v>0</v>
+        <v>11201</v>
       </c>
       <c r="E21" s="6">
         <v>0</v>
@@ -3971,24 +4219,24 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="A22" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="72"/>
       <c r="C22" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D22" s="6">
-        <v>0</v>
+        <v>11202</v>
       </c>
       <c r="E22" s="6">
         <v>0</v>
@@ -3998,53 +4246,53 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="A23" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B23" s="72"/>
       <c r="C23" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D23" s="6">
-        <v>0</v>
+        <v>11203</v>
       </c>
       <c r="E23" s="6">
         <v>1</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13">
       <c r="A24" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" s="72"/>
       <c r="C24" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D24" s="6">
-        <v>0</v>
+        <v>11204</v>
       </c>
       <c r="E24" s="6">
         <v>0</v>
@@ -4054,24 +4302,24 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B25" s="72"/>
       <c r="C25" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D25" s="6">
-        <v>0</v>
+        <v>11205</v>
       </c>
       <c r="E25" s="6">
         <v>0</v>
@@ -4081,24 +4329,24 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13">
       <c r="A26" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="72"/>
       <c r="C26" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D26" s="6">
-        <v>0</v>
+        <v>11206</v>
       </c>
       <c r="E26" s="6">
         <v>0</v>
@@ -4108,24 +4356,24 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13">
       <c r="A27" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B27" s="72"/>
       <c r="C27" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D27" s="6">
-        <v>0</v>
+        <v>11207</v>
       </c>
       <c r="E27" s="6">
         <v>0</v>
@@ -4135,24 +4383,24 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="A28" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B28" s="72"/>
       <c r="C28" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D28" s="6">
-        <v>0</v>
+        <v>11208</v>
       </c>
       <c r="E28" s="6">
         <v>0</v>
@@ -4162,24 +4410,24 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B29" s="72"/>
       <c r="C29" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D29" s="6">
-        <v>0</v>
+        <v>11209</v>
       </c>
       <c r="E29" s="6">
         <v>0</v>
@@ -4189,24 +4437,24 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" s="72"/>
       <c r="C30" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D30" s="6">
-        <v>0</v>
+        <v>11210</v>
       </c>
       <c r="E30" s="6">
         <v>0</v>
@@ -4216,24 +4464,24 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="A31" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B31" s="72"/>
       <c r="C31" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D31" s="6">
-        <v>0</v>
+        <v>11211</v>
       </c>
       <c r="E31" s="6">
         <v>0</v>
@@ -4243,24 +4491,24 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="A32" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B32" s="72"/>
       <c r="C32" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D32" s="6">
-        <v>0</v>
+        <v>11212</v>
       </c>
       <c r="E32" s="6">
         <v>0</v>
@@ -4270,24 +4518,24 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13">
       <c r="A33" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B33" s="72"/>
       <c r="C33" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D33" s="6">
-        <v>0</v>
+        <v>11213</v>
       </c>
       <c r="E33" s="6">
         <v>0</v>
@@ -4297,24 +4545,24 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13">
       <c r="A34" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B34" s="72"/>
       <c r="C34" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D34" s="6">
-        <v>0</v>
+        <v>11214</v>
       </c>
       <c r="E34" s="6">
         <v>0</v>
@@ -4324,47 +4572,47 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="28">
       <c r="A35" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" s="72" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D35" s="6">
-        <v>1</v>
+        <v>11299</v>
       </c>
       <c r="E35" s="6">
         <v>4</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J35" s="22" t="s">
         <v>60</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -4384,7 +4632,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="19.4140625" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
@@ -4392,7 +4640,7 @@
     <col min="4" max="4" width="138.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="27" t="s">
         <v>40</v>
       </c>
@@ -4406,19 +4654,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="66" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="66" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
@@ -4426,125 +4674,125 @@
         <v>76</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="83" customHeight="1" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="83" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C4" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="179" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="179" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>166</v>
-      </c>
       <c r="D5" s="68" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="53" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="53" customFormat="1" ht="48" customHeight="1">
       <c r="A6" s="50"/>
       <c r="B6" s="50"/>
       <c r="C6" s="51"/>
       <c r="D6" s="52"/>
     </row>
-    <row r="7" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="43.5" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="7"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="7"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="7"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="7"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="7"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="7"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="7"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="7"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="7"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="7"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="7"/>
@@ -4559,54 +4807,648 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="78.08203125" customWidth="1"/>
-    <col min="2" max="2" width="45.58203125" customWidth="1"/>
+    <col min="1" max="1" width="42.9140625" customWidth="1"/>
+    <col min="2" max="2" width="29.9140625" customWidth="1"/>
+    <col min="3" max="3" width="42.25" customWidth="1"/>
+    <col min="4" max="4" width="14.9140625" customWidth="1"/>
+    <col min="5" max="5" width="14.4140625" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="110.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="1" spans="1:6" ht="59.5" customHeight="1">
+      <c r="A1" s="79" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="94" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="95"/>
+      <c r="F1" s="80" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="86">
+        <v>1</v>
+      </c>
+      <c r="B2" s="81">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="96" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="86">
+        <v>1</v>
+      </c>
+      <c r="B3" s="81">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6">
+        <v>9</v>
+      </c>
+      <c r="F3" s="97"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="86">
+        <v>1</v>
+      </c>
+      <c r="B4" s="81">
+        <v>1</v>
+      </c>
+      <c r="C4" s="82">
+        <v>1</v>
+      </c>
+      <c r="D4" s="82">
+        <v>0</v>
+      </c>
+      <c r="E4" s="82">
+        <v>0</v>
+      </c>
+      <c r="F4" s="98" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="86">
+        <v>1</v>
+      </c>
+      <c r="B5" s="81">
+        <v>1</v>
+      </c>
+      <c r="C5" s="82">
+        <v>1</v>
+      </c>
+      <c r="D5" s="82">
+        <v>9</v>
+      </c>
+      <c r="E5" s="82">
+        <v>9</v>
+      </c>
+      <c r="F5" s="99"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="86">
+        <v>1</v>
+      </c>
+      <c r="B6" s="81">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="92" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="86">
+        <v>1</v>
+      </c>
+      <c r="B7" s="81">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6">
+        <v>9</v>
+      </c>
+      <c r="E7" s="6">
+        <v>9</v>
+      </c>
+      <c r="F7" s="93"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="86">
+        <v>1</v>
+      </c>
+      <c r="B8" s="81">
+        <v>1</v>
+      </c>
+      <c r="C8" s="82">
+        <v>3</v>
+      </c>
+      <c r="D8" s="82">
+        <v>0</v>
+      </c>
+      <c r="E8" s="82">
+        <v>0</v>
+      </c>
+      <c r="F8" s="90" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="86">
+        <v>1</v>
+      </c>
+      <c r="B9" s="81">
+        <v>1</v>
+      </c>
+      <c r="C9" s="82">
+        <v>3</v>
+      </c>
+      <c r="D9" s="82">
+        <v>9</v>
+      </c>
+      <c r="E9" s="82">
+        <v>9</v>
+      </c>
+      <c r="F9" s="91"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="86">
+        <v>1</v>
+      </c>
+      <c r="B10" s="81">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="92" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="86">
+        <v>1</v>
+      </c>
+      <c r="B11" s="81">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6">
+        <v>9</v>
+      </c>
+      <c r="E11" s="6">
+        <v>9</v>
+      </c>
+      <c r="F11" s="93"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="86">
+        <v>1</v>
+      </c>
+      <c r="B12" s="81">
+        <v>1</v>
+      </c>
+      <c r="C12" s="83" t="s">
+        <v>228</v>
+      </c>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="91" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="86">
+        <v>1</v>
+      </c>
+      <c r="B13" s="81">
+        <v>1</v>
+      </c>
+      <c r="C13" s="83" t="s">
+        <v>216</v>
+      </c>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="91"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="86">
+        <v>1</v>
+      </c>
+      <c r="B14" s="84">
+        <v>2</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="92" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="86">
+        <v>1</v>
+      </c>
+      <c r="B15" s="84">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>9</v>
+      </c>
+      <c r="E15" s="6">
+        <v>9</v>
+      </c>
+      <c r="F15" s="93"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="86">
+        <v>1</v>
+      </c>
+      <c r="B16" s="84">
+        <v>2</v>
+      </c>
+      <c r="C16" s="82">
+        <v>1</v>
+      </c>
+      <c r="D16" s="82">
+        <v>0</v>
+      </c>
+      <c r="E16" s="82">
+        <v>0</v>
+      </c>
+      <c r="F16" s="90" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="86">
+        <v>1</v>
+      </c>
+      <c r="B17" s="84">
+        <v>2</v>
+      </c>
+      <c r="C17" s="82">
+        <v>1</v>
+      </c>
+      <c r="D17" s="82">
+        <v>9</v>
+      </c>
+      <c r="E17" s="82">
+        <v>9</v>
+      </c>
+      <c r="F17" s="91"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="86">
+        <v>1</v>
+      </c>
+      <c r="B18" s="84">
+        <v>2</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" s="92" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="86">
+        <v>1</v>
+      </c>
+      <c r="B19" s="84">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6">
+        <v>9</v>
+      </c>
+      <c r="E19" s="6">
+        <v>9</v>
+      </c>
+      <c r="F19" s="93"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="86">
+        <v>1</v>
+      </c>
+      <c r="B20" s="84">
+        <v>2</v>
+      </c>
+      <c r="C20" s="82">
+        <v>3</v>
+      </c>
+      <c r="D20" s="82">
+        <v>0</v>
+      </c>
+      <c r="E20" s="82">
+        <v>0</v>
+      </c>
+      <c r="F20" s="90" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="86">
+        <v>1</v>
+      </c>
+      <c r="B21" s="84">
+        <v>2</v>
+      </c>
+      <c r="C21" s="82">
+        <v>3</v>
+      </c>
+      <c r="D21" s="82">
+        <v>9</v>
+      </c>
+      <c r="E21" s="82">
+        <v>9</v>
+      </c>
+      <c r="F21" s="91"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="86">
+        <v>1</v>
+      </c>
+      <c r="B22" s="85">
+        <v>3</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+      <c r="F22" s="92" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="86">
+        <v>1</v>
+      </c>
+      <c r="B23" s="85">
+        <v>3</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6">
+        <v>9</v>
+      </c>
+      <c r="E23" s="6">
+        <v>9</v>
+      </c>
+      <c r="F23" s="93"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="86">
+        <v>1</v>
+      </c>
+      <c r="B24" s="85">
+        <v>3</v>
+      </c>
+      <c r="C24" s="82">
+        <v>1</v>
+      </c>
+      <c r="D24" s="82">
+        <v>0</v>
+      </c>
+      <c r="E24" s="82">
+        <v>0</v>
+      </c>
+      <c r="F24" s="90" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="86">
+        <v>1</v>
+      </c>
+      <c r="B25" s="85">
+        <v>3</v>
+      </c>
+      <c r="C25" s="82">
+        <v>1</v>
+      </c>
+      <c r="D25" s="82">
+        <v>9</v>
+      </c>
+      <c r="E25" s="82">
+        <v>9</v>
+      </c>
+      <c r="F25" s="91"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="86">
+        <v>1</v>
+      </c>
+      <c r="B26" s="85">
+        <v>3</v>
+      </c>
+      <c r="C26" s="6">
+        <v>2</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0</v>
+      </c>
+      <c r="F26" s="92" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="86">
+        <v>1</v>
+      </c>
+      <c r="B27" s="85">
+        <v>3</v>
+      </c>
+      <c r="C27" s="6">
+        <v>2</v>
+      </c>
+      <c r="D27" s="6">
+        <v>9</v>
+      </c>
+      <c r="E27" s="6">
+        <v>9</v>
+      </c>
+      <c r="F27" s="93"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="86">
+        <v>1</v>
+      </c>
+      <c r="B28" s="85">
+        <v>3</v>
+      </c>
+      <c r="C28" s="82">
+        <v>3</v>
+      </c>
+      <c r="D28" s="82">
+        <v>0</v>
+      </c>
+      <c r="E28" s="82">
+        <v>0</v>
+      </c>
+      <c r="F28" s="90" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="86">
+        <v>1</v>
+      </c>
+      <c r="B29" s="85">
+        <v>3</v>
+      </c>
+      <c r="C29" s="82">
+        <v>3</v>
+      </c>
+      <c r="D29" s="82">
+        <v>9</v>
+      </c>
+      <c r="E29" s="82">
+        <v>9</v>
+      </c>
+      <c r="F29" s="91"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="86">
+        <v>1</v>
+      </c>
+      <c r="B30" s="85">
+        <v>3</v>
+      </c>
+      <c r="C30" s="6">
+        <v>4</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0</v>
+      </c>
+      <c r="F30" s="92" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="86">
+        <v>1</v>
+      </c>
+      <c r="B31" s="85">
+        <v>3</v>
+      </c>
+      <c r="C31" s="6">
+        <v>4</v>
+      </c>
+      <c r="D31" s="6">
+        <v>9</v>
+      </c>
+      <c r="E31" s="6">
+        <v>9</v>
+      </c>
+      <c r="F31" s="93"/>
+    </row>
+    <row r="46" spans="1:2" ht="84.5">
+      <c r="A46" s="87" t="s">
+        <v>234</v>
+      </c>
+      <c r="B46" s="88"/>
+    </row>
+    <row r="47" spans="1:2" ht="74">
+      <c r="A47" s="89" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" s="88"/>
+    </row>
+    <row r="48" spans="1:2" ht="95">
+      <c r="A48" s="89" t="s">
+        <v>235</v>
+      </c>
+      <c r="B48" s="88"/>
+    </row>
+    <row r="49" spans="1:2" ht="147.5">
+      <c r="A49" s="89" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="196" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>180</v>
+      <c r="B49" s="89" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F22:F23"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modify the output1 string of disconnection.
</commit_message>
<xml_diff>
--- a/config/Config.xlsx
+++ b/config/Config.xlsx
@@ -700,11 +700,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">07-04 00:05:20.386 13334 13334 I wpa_supplicant: wlan0: CTRL-EVENT-DISCONNECTED bssid=18:31:bf:a8:ef:60 reason=3 locally_generated=1 disconnect_rssi=0
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>VAL4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1924,6 +1919,11 @@
   </si>
   <si>
     <t>PROCESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CTRL-EVENT-DISCONNECTED bssid=&lt;VAL1&gt; reason=&lt;VAL2&gt; locally_generated=&lt;VAL3&gt; disconnect_rssi=&lt;VAL4&gt;
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2414,6 +2414,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2436,12 +2442,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2738,10 +2738,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="70" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2749,7 +2749,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2757,7 +2757,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2765,7 +2765,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2773,7 +2773,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2781,7 +2781,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2789,7 +2789,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2815,10 +2815,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="70" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2826,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2834,7 +2834,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2842,7 +2842,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2850,7 +2850,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2858,7 +2858,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2866,7 +2866,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2905,13 +2905,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>64</v>
@@ -2946,7 +2946,7 @@
         <v>80</v>
       </c>
       <c r="B2" s="72" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>55</v>
@@ -2958,15 +2958,15 @@
         <v>1</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>50</v>
@@ -2980,7 +2980,7 @@
         <v>81</v>
       </c>
       <c r="B3" s="73" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C3" s="58" t="s">
         <v>3</v>
@@ -3012,7 +3012,7 @@
         <v>82</v>
       </c>
       <c r="B4" s="72" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>2</v>
@@ -3024,7 +3024,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>61</v>
@@ -3033,7 +3033,7 @@
         <v>50</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>5</v>
@@ -3044,7 +3044,7 @@
         <v>83</v>
       </c>
       <c r="B5" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>59</v>
@@ -3069,7 +3069,7 @@
         <v>8</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
@@ -3528,8 +3528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3554,13 +3554,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>64</v>
@@ -3575,7 +3575,7 @@
         <v>56</v>
       </c>
       <c r="I1" s="69" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J1" s="24" t="s">
         <v>65</v>
@@ -3598,10 +3598,10 @@
         <v>84</v>
       </c>
       <c r="B2" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D2" s="26">
         <v>11200</v>
@@ -3614,7 +3614,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>10</v>
@@ -3629,7 +3629,7 @@
         <v>106</v>
       </c>
       <c r="B3" s="72" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>28</v>
@@ -3641,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -3662,7 +3662,7 @@
         <v>97</v>
       </c>
       <c r="B4" s="72" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>68</v>
@@ -3674,7 +3674,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -3695,7 +3695,7 @@
         <v>104</v>
       </c>
       <c r="B5" s="72" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>71</v>
@@ -3707,7 +3707,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -3728,7 +3728,7 @@
         <v>85</v>
       </c>
       <c r="B6" s="72" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>73</v>
@@ -3759,10 +3759,10 @@
         <v>86</v>
       </c>
       <c r="B7" s="72" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" s="26">
         <v>11205</v>
@@ -3771,20 +3771,20 @@
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L7" s="15"/>
       <c r="M7" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3792,7 +3792,7 @@
         <v>86</v>
       </c>
       <c r="B8" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>38</v>
@@ -3823,10 +3823,10 @@
         <v>87</v>
       </c>
       <c r="B9" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D9" s="26">
         <v>11207</v>
@@ -3857,10 +3857,10 @@
         <v>88</v>
       </c>
       <c r="B10" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10" s="26">
         <v>11208</v>
@@ -3890,7 +3890,7 @@
         <v>89</v>
       </c>
       <c r="B11" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>16</v>
@@ -3921,7 +3921,7 @@
         <v>90</v>
       </c>
       <c r="B12" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>20</v>
@@ -3952,7 +3952,7 @@
         <v>105</v>
       </c>
       <c r="B13" s="72" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="49" t="s">
         <v>78</v>
@@ -3964,7 +3964,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -3988,7 +3988,7 @@
         <v>91</v>
       </c>
       <c r="B14" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>79</v>
@@ -4019,7 +4019,7 @@
         <v>92</v>
       </c>
       <c r="B15" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>100</v>
@@ -4050,7 +4050,7 @@
         <v>93</v>
       </c>
       <c r="B16" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>102</v>
@@ -4081,7 +4081,7 @@
         <v>94</v>
       </c>
       <c r="B17" s="72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>103</v>
@@ -4112,7 +4112,7 @@
         <v>95</v>
       </c>
       <c r="B18" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>36</v>
@@ -4124,10 +4124,10 @@
         <v>1</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
@@ -4147,13 +4147,13 @@
         <v>96</v>
       </c>
       <c r="B19" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C19" s="66" t="s">
         <v>117</v>
       </c>
       <c r="D19" s="67" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E19" s="6">
         <v>0</v>
@@ -4178,7 +4178,7 @@
         <v>109</v>
       </c>
       <c r="B20" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>116</v>
@@ -4194,7 +4194,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>118</v>
@@ -4210,7 +4210,7 @@
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D21" s="6">
         <v>11301</v>
@@ -4223,10 +4223,10 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="B22" s="72"/>
       <c r="C22" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D22" s="6">
         <v>11302</v>
@@ -4250,10 +4250,10 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="B23" s="72"/>
       <c r="C23" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D23" s="6">
         <v>11303</v>
@@ -4273,16 +4273,16 @@
         <v>1</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -4293,7 +4293,7 @@
       </c>
       <c r="B24" s="72"/>
       <c r="C24" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D24" s="6">
         <v>11304</v>
@@ -4306,10 +4306,10 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="B25" s="72"/>
       <c r="C25" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D25" s="6">
         <v>11305</v>
@@ -4333,10 +4333,10 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="B26" s="72"/>
       <c r="C26" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D26" s="6">
         <v>11306</v>
@@ -4360,21 +4360,21 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B27" s="72"/>
       <c r="C27" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D27" s="6">
         <v>11307</v>
@@ -4387,21 +4387,21 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B28" s="72"/>
       <c r="C28" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D28" s="6">
         <v>11308</v>
@@ -4414,21 +4414,21 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" s="72"/>
       <c r="C29" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D29" s="6">
         <v>11309</v>
@@ -4441,21 +4441,21 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B30" s="72"/>
       <c r="C30" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D30" s="6">
         <v>11310</v>
@@ -4468,21 +4468,21 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B31" s="72"/>
       <c r="C31" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D31" s="6">
         <v>11311</v>
@@ -4495,21 +4495,21 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B32" s="72"/>
       <c r="C32" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D32" s="6">
         <v>11312</v>
@@ -4522,21 +4522,21 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B33" s="72"/>
       <c r="C33" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D33" s="6">
         <v>11313</v>
@@ -4549,21 +4549,21 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B34" s="72"/>
       <c r="C34" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D34" s="6">
         <v>11314</v>
@@ -4576,23 +4576,23 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B35" s="72" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D35" s="6">
         <v>11399</v>
@@ -4601,22 +4601,22 @@
         <v>4</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J35" s="22" t="s">
         <v>60</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>122</v>
+        <v>235</v>
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -4663,10 +4663,10 @@
         <v>43</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -4678,10 +4678,10 @@
         <v>75</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="83" customHeight="1" x14ac:dyDescent="0.3">
@@ -4692,24 +4692,24 @@
         <v>75</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="179" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="64" t="s">
         <v>121</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D5" s="68" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="53" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
@@ -4829,20 +4829,20 @@
   <sheetData>
     <row r="1" spans="1:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="79" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B1" s="79" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="94" t="s">
         <v>210</v>
       </c>
-      <c r="C1" s="79" t="s">
-        <v>229</v>
-      </c>
-      <c r="D1" s="92" t="s">
+      <c r="E1" s="95"/>
+      <c r="F1" s="80" t="s">
         <v>211</v>
-      </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="80" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4861,8 +4861,8 @@
       <c r="E2" s="6">
         <v>0</v>
       </c>
-      <c r="F2" s="94" t="s">
-        <v>230</v>
+      <c r="F2" s="96" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -4881,7 +4881,7 @@
       <c r="E3" s="6">
         <v>9</v>
       </c>
-      <c r="F3" s="95"/>
+      <c r="F3" s="97"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="86">
@@ -4899,8 +4899,8 @@
       <c r="E4" s="82">
         <v>0</v>
       </c>
-      <c r="F4" s="96" t="s">
-        <v>231</v>
+      <c r="F4" s="98" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -4919,7 +4919,7 @@
       <c r="E5" s="82">
         <v>9</v>
       </c>
-      <c r="F5" s="97"/>
+      <c r="F5" s="99"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="86">
@@ -4937,8 +4937,8 @@
       <c r="E6" s="6">
         <v>0</v>
       </c>
-      <c r="F6" s="90" t="s">
-        <v>224</v>
+      <c r="F6" s="92" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -4957,7 +4957,7 @@
       <c r="E7" s="6">
         <v>9</v>
       </c>
-      <c r="F7" s="91"/>
+      <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="86">
@@ -4975,8 +4975,8 @@
       <c r="E8" s="82">
         <v>0</v>
       </c>
-      <c r="F8" s="98" t="s">
-        <v>213</v>
+      <c r="F8" s="90" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -4995,7 +4995,7 @@
       <c r="E9" s="82">
         <v>9</v>
       </c>
-      <c r="F9" s="99"/>
+      <c r="F9" s="91"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="86">
@@ -5013,8 +5013,8 @@
       <c r="E10" s="6">
         <v>0</v>
       </c>
-      <c r="F10" s="90" t="s">
-        <v>225</v>
+      <c r="F10" s="92" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -5033,7 +5033,7 @@
       <c r="E11" s="6">
         <v>9</v>
       </c>
-      <c r="F11" s="91"/>
+      <c r="F11" s="93"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="86">
@@ -5043,12 +5043,12 @@
         <v>1</v>
       </c>
       <c r="C12" s="83" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D12" s="82"/>
       <c r="E12" s="82"/>
-      <c r="F12" s="99" t="s">
-        <v>215</v>
+      <c r="F12" s="91" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -5059,11 +5059,11 @@
         <v>1</v>
       </c>
       <c r="C13" s="83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D13" s="82"/>
       <c r="E13" s="82"/>
-      <c r="F13" s="99"/>
+      <c r="F13" s="91"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="86">
@@ -5081,8 +5081,8 @@
       <c r="E14" s="6">
         <v>0</v>
       </c>
-      <c r="F14" s="90" t="s">
-        <v>227</v>
+      <c r="F14" s="92" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -5101,7 +5101,7 @@
       <c r="E15" s="6">
         <v>9</v>
       </c>
-      <c r="F15" s="91"/>
+      <c r="F15" s="93"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="86">
@@ -5119,8 +5119,8 @@
       <c r="E16" s="82">
         <v>0</v>
       </c>
-      <c r="F16" s="98" t="s">
-        <v>228</v>
+      <c r="F16" s="90" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -5139,7 +5139,7 @@
       <c r="E17" s="82">
         <v>9</v>
       </c>
-      <c r="F17" s="99"/>
+      <c r="F17" s="91"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="86">
@@ -5157,8 +5157,8 @@
       <c r="E18" s="6">
         <v>0</v>
       </c>
-      <c r="F18" s="90" t="s">
-        <v>216</v>
+      <c r="F18" s="92" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -5177,7 +5177,7 @@
       <c r="E19" s="6">
         <v>9</v>
       </c>
-      <c r="F19" s="91"/>
+      <c r="F19" s="93"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="86">
@@ -5195,8 +5195,8 @@
       <c r="E20" s="82">
         <v>0</v>
       </c>
-      <c r="F20" s="98" t="s">
-        <v>217</v>
+      <c r="F20" s="90" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -5215,7 +5215,7 @@
       <c r="E21" s="82">
         <v>9</v>
       </c>
-      <c r="F21" s="99"/>
+      <c r="F21" s="91"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="86">
@@ -5233,8 +5233,8 @@
       <c r="E22" s="6">
         <v>0</v>
       </c>
-      <c r="F22" s="90" t="s">
-        <v>218</v>
+      <c r="F22" s="92" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -5253,7 +5253,7 @@
       <c r="E23" s="6">
         <v>9</v>
       </c>
-      <c r="F23" s="91"/>
+      <c r="F23" s="93"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="86">
@@ -5271,8 +5271,8 @@
       <c r="E24" s="82">
         <v>0</v>
       </c>
-      <c r="F24" s="98" t="s">
-        <v>219</v>
+      <c r="F24" s="90" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -5291,7 +5291,7 @@
       <c r="E25" s="82">
         <v>9</v>
       </c>
-      <c r="F25" s="99"/>
+      <c r="F25" s="91"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="86">
@@ -5309,8 +5309,8 @@
       <c r="E26" s="6">
         <v>0</v>
       </c>
-      <c r="F26" s="90" t="s">
-        <v>220</v>
+      <c r="F26" s="92" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -5329,7 +5329,7 @@
       <c r="E27" s="6">
         <v>9</v>
       </c>
-      <c r="F27" s="91"/>
+      <c r="F27" s="93"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="86">
@@ -5347,8 +5347,8 @@
       <c r="E28" s="82">
         <v>0</v>
       </c>
-      <c r="F28" s="98" t="s">
-        <v>221</v>
+      <c r="F28" s="90" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -5367,7 +5367,7 @@
       <c r="E29" s="82">
         <v>9</v>
       </c>
-      <c r="F29" s="99"/>
+      <c r="F29" s="91"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="86">
@@ -5385,8 +5385,8 @@
       <c r="E30" s="6">
         <v>0</v>
       </c>
-      <c r="F30" s="90" t="s">
-        <v>222</v>
+      <c r="F30" s="92" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -5405,36 +5405,42 @@
       <c r="E31" s="6">
         <v>9</v>
       </c>
-      <c r="F31" s="91"/>
+      <c r="F31" s="93"/>
     </row>
     <row r="46" spans="1:2" ht="84.5" x14ac:dyDescent="0.3">
       <c r="A46" s="87" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B46" s="88"/>
     </row>
     <row r="47" spans="1:2" ht="74" x14ac:dyDescent="0.3">
       <c r="A47" s="89" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B47" s="88"/>
     </row>
     <row r="48" spans="1:2" ht="95" x14ac:dyDescent="0.3">
       <c r="A48" s="89" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B48" s="88"/>
     </row>
     <row r="49" spans="1:2" ht="147.5" x14ac:dyDescent="0.3">
       <c r="A49" s="89" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B49" s="89" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="F28:F29"/>
@@ -5445,12 +5451,6 @@
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify output string of disconnection.
</commit_message>
<xml_diff>
--- a/config/Config.xlsx
+++ b/config/Config.xlsx
@@ -1922,8 +1922,98 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">CTRL-EVENT-DISCONNECTED bssid=&lt;VAL1&gt; reason=&lt;VAL2&gt; locally_generated=&lt;VAL3&gt; disconnect_rssi=&lt;VAL4&gt;
+    <r>
+      <t>CTRL-EVENT-DISCONNECTED bssid=&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VAL1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; reason=&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VAL2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; locally_generated=&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VAL3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; disconnect_rssi=&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VAL4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;
 </t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1931,7 +2021,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2414,34 +2504,34 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2730,13 +2820,13 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="70" t="s">
         <v>176</v>
       </c>
@@ -2744,7 +2834,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2752,7 +2842,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2760,7 +2850,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2768,7 +2858,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2776,7 +2866,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2784,7 +2874,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2807,13 +2897,13 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="13.25" customWidth="1"/>
     <col min="2" max="2" width="23.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="70" t="s">
         <v>176</v>
       </c>
@@ -2821,7 +2911,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2829,7 +2919,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2837,7 +2927,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2845,7 +2935,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2853,7 +2943,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2861,7 +2951,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2884,7 +2974,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="16.4140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="16.4140625" style="77" customWidth="1"/>
@@ -2900,7 +2990,7 @@
     <col min="13" max="13" width="127.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="15.5">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2941,7 +3031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="57" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="57" customFormat="1" ht="76" customHeight="1">
       <c r="A2" s="55" t="s">
         <v>80</v>
       </c>
@@ -2975,7 +3065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="57" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="57" customFormat="1" ht="76" customHeight="1">
       <c r="A3" s="55" t="s">
         <v>81</v>
       </c>
@@ -3007,7 +3097,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="11" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="11" customFormat="1" ht="76" customHeight="1">
       <c r="A4" s="55" t="s">
         <v>82</v>
       </c>
@@ -3039,7 +3129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="11" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="11" customFormat="1" ht="73.5" customHeight="1">
       <c r="A5" s="55" t="s">
         <v>83</v>
       </c>
@@ -3072,7 +3162,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1">
       <c r="A6" s="35"/>
       <c r="B6" s="74"/>
       <c r="C6" s="36"/>
@@ -3083,7 +3173,7 @@
       <c r="H6" s="16"/>
       <c r="L6" s="41"/>
     </row>
-    <row r="7" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1">
       <c r="A7" s="35"/>
       <c r="B7" s="74"/>
       <c r="C7" s="36"/>
@@ -3096,29 +3186,29 @@
       <c r="K7" s="42"/>
       <c r="L7" s="41"/>
     </row>
-    <row r="8" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="40" customFormat="1" ht="76" customHeight="1">
       <c r="B8" s="75"/>
       <c r="C8" s="41"/>
       <c r="D8" s="43"/>
       <c r="F8" s="44"/>
       <c r="L8" s="41"/>
     </row>
-    <row r="9" spans="1:13" ht="76" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="76" customHeight="1">
       <c r="A9"/>
       <c r="B9" s="76"/>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="39" customHeight="1">
       <c r="A10"/>
       <c r="B10" s="76"/>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="39" customHeight="1">
       <c r="A11"/>
       <c r="B11" s="76"/>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="1" customFormat="1">
       <c r="A12"/>
       <c r="B12" s="76"/>
       <c r="C12" s="9"/>
@@ -3132,387 +3222,387 @@
       <c r="K12"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13"/>
       <c r="B13" s="76"/>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14"/>
       <c r="B14" s="76"/>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15"/>
       <c r="B15" s="76"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16"/>
       <c r="B16" s="76"/>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17"/>
       <c r="B17" s="76"/>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18"/>
       <c r="B18" s="76"/>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19"/>
       <c r="B19" s="76"/>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20"/>
       <c r="B20" s="76"/>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21"/>
       <c r="B21" s="76"/>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22"/>
       <c r="B22" s="76"/>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23"/>
       <c r="B23" s="76"/>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24"/>
       <c r="B24" s="76"/>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25"/>
       <c r="B25" s="76"/>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26"/>
       <c r="B26" s="76"/>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27"/>
       <c r="B27" s="76"/>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28"/>
       <c r="B28" s="76"/>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29"/>
       <c r="B29" s="76"/>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5">
       <c r="A30"/>
       <c r="B30" s="76"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5">
       <c r="A31"/>
       <c r="B31" s="76"/>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5">
       <c r="A32"/>
       <c r="B32" s="76"/>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5">
       <c r="A33"/>
       <c r="B33" s="76"/>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5">
       <c r="A34"/>
       <c r="B34" s="76"/>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35"/>
       <c r="B35" s="76"/>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36"/>
       <c r="B36" s="76"/>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37"/>
       <c r="B37" s="76"/>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5">
       <c r="A38"/>
       <c r="B38" s="76"/>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5">
       <c r="A39"/>
       <c r="B39" s="76"/>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40"/>
       <c r="B40" s="76"/>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5">
       <c r="A41"/>
       <c r="B41" s="76"/>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5">
       <c r="A42"/>
       <c r="B42" s="76"/>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5">
       <c r="A43"/>
       <c r="B43" s="76"/>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5">
       <c r="A44"/>
       <c r="B44" s="76"/>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5">
       <c r="A45"/>
       <c r="B45" s="76"/>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5">
       <c r="A46"/>
       <c r="B46" s="76"/>
       <c r="E46"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5">
       <c r="A47"/>
       <c r="B47" s="76"/>
       <c r="E47"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5">
       <c r="A48"/>
       <c r="B48" s="76"/>
       <c r="E48"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5">
       <c r="A49"/>
       <c r="B49" s="76"/>
       <c r="E49"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5">
       <c r="A50"/>
       <c r="B50" s="76"/>
       <c r="E50"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5">
       <c r="A51"/>
       <c r="B51" s="76"/>
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5">
       <c r="A52"/>
       <c r="B52" s="76"/>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5">
       <c r="A53"/>
       <c r="B53" s="76"/>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5">
       <c r="A54"/>
       <c r="B54" s="76"/>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5">
       <c r="A55"/>
       <c r="B55" s="76"/>
       <c r="E55"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5">
       <c r="A56"/>
       <c r="B56" s="76"/>
       <c r="E56"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5">
       <c r="A57"/>
       <c r="B57" s="76"/>
       <c r="E57"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5">
       <c r="A58"/>
       <c r="B58" s="76"/>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5">
       <c r="A59"/>
       <c r="B59" s="76"/>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5">
       <c r="A60"/>
       <c r="B60" s="76"/>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5">
       <c r="A61"/>
       <c r="B61" s="76"/>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5">
       <c r="A62"/>
       <c r="B62" s="76"/>
       <c r="E62"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5">
       <c r="A63"/>
       <c r="B63" s="76"/>
       <c r="E63"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5">
       <c r="A64"/>
       <c r="B64" s="76"/>
       <c r="E64"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5">
       <c r="A65"/>
       <c r="B65" s="76"/>
       <c r="E65"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5">
       <c r="A66"/>
       <c r="B66" s="76"/>
       <c r="E66"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5">
       <c r="A67"/>
       <c r="B67" s="76"/>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5">
       <c r="A68"/>
       <c r="B68" s="76"/>
       <c r="E68"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5">
       <c r="A69"/>
       <c r="B69" s="76"/>
       <c r="E69"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5">
       <c r="A70"/>
       <c r="B70" s="76"/>
       <c r="E70"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5">
       <c r="A71"/>
       <c r="B71" s="76"/>
       <c r="E71"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5">
       <c r="A72"/>
       <c r="B72" s="76"/>
       <c r="E72"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5">
       <c r="A73"/>
       <c r="B73" s="76"/>
       <c r="E73"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5">
       <c r="A74"/>
       <c r="B74" s="76"/>
       <c r="E74"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5">
       <c r="A75"/>
       <c r="B75" s="76"/>
       <c r="E75"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5">
       <c r="A76"/>
       <c r="B76" s="76"/>
       <c r="E76"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5">
       <c r="A77"/>
       <c r="B77" s="76"/>
       <c r="E77"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5">
       <c r="A78"/>
       <c r="B78" s="76"/>
       <c r="E78"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5">
       <c r="A79"/>
       <c r="B79" s="76"/>
       <c r="E79"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5">
       <c r="A80"/>
       <c r="B80" s="76"/>
       <c r="E80"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5">
       <c r="A81"/>
       <c r="B81" s="76"/>
       <c r="E81"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5">
       <c r="A82"/>
       <c r="B82" s="76"/>
       <c r="E82"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5">
       <c r="A83"/>
       <c r="B83" s="76"/>
       <c r="E83"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5">
       <c r="A84"/>
       <c r="B84" s="76"/>
       <c r="E84"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5">
       <c r="A85"/>
       <c r="B85" s="76"/>
       <c r="E85"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5">
       <c r="A86"/>
       <c r="B86" s="76"/>
       <c r="E86"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5">
       <c r="A87"/>
       <c r="B87" s="76"/>
       <c r="E87"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5">
       <c r="A88"/>
       <c r="B88" s="76"/>
       <c r="E88"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5">
       <c r="A89"/>
       <c r="B89" s="76"/>
       <c r="E89"/>
@@ -3528,11 +3618,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="J22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="21" style="78" customWidth="1"/>
@@ -3549,7 +3639,7 @@
     <col min="14" max="14" width="64.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="15.5">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3593,7 +3683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="34.5" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>84</v>
       </c>
@@ -3624,7 +3714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="34.5" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>106</v>
       </c>
@@ -3657,7 +3747,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="39" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>97</v>
       </c>
@@ -3690,7 +3780,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="36" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>104</v>
       </c>
@@ -3723,7 +3813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="24" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>85</v>
       </c>
@@ -3754,7 +3844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="24" customHeight="1">
       <c r="A7" s="65" t="s">
         <v>86</v>
       </c>
@@ -3787,7 +3877,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="25.5" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>86</v>
       </c>
@@ -3818,7 +3908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="25.5" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>87</v>
       </c>
@@ -3852,7 +3942,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="25.5" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>88</v>
       </c>
@@ -3885,7 +3975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="25.5" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>89</v>
       </c>
@@ -3916,7 +4006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="25.5" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>90</v>
       </c>
@@ -3947,7 +4037,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="25.5" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>105</v>
       </c>
@@ -3983,7 +4073,7 @@
       </c>
       <c r="N13" s="21"/>
     </row>
-    <row r="14" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="29" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>91</v>
       </c>
@@ -4014,7 +4104,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="46" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>92</v>
       </c>
@@ -4045,7 +4135,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="46" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>93</v>
       </c>
@@ -4076,7 +4166,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="46" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>94</v>
       </c>
@@ -4107,7 +4197,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="42">
       <c r="A18" s="10" t="s">
         <v>95</v>
       </c>
@@ -4142,7 +4232,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="42">
       <c r="A19" s="65" t="s">
         <v>96</v>
       </c>
@@ -4173,7 +4263,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="56" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="56">
       <c r="A20" s="10" t="s">
         <v>109</v>
       </c>
@@ -4204,7 +4294,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13">
       <c r="A21" s="10" t="s">
         <v>110</v>
       </c>
@@ -4231,7 +4321,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="A22" s="10" t="s">
         <v>111</v>
       </c>
@@ -4258,7 +4348,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="A23" s="10" t="s">
         <v>112</v>
       </c>
@@ -4287,7 +4377,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13">
       <c r="A24" s="10" t="s">
         <v>113</v>
       </c>
@@ -4314,7 +4404,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25" s="10" t="s">
         <v>114</v>
       </c>
@@ -4341,7 +4431,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13">
       <c r="A26" s="10" t="s">
         <v>115</v>
       </c>
@@ -4368,7 +4458,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13">
       <c r="A27" s="10" t="s">
         <v>140</v>
       </c>
@@ -4395,7 +4485,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="A28" s="10" t="s">
         <v>141</v>
       </c>
@@ -4422,7 +4512,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29" s="10" t="s">
         <v>142</v>
       </c>
@@ -4449,7 +4539,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30" s="10" t="s">
         <v>143</v>
       </c>
@@ -4476,7 +4566,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="A31" s="10" t="s">
         <v>144</v>
       </c>
@@ -4503,7 +4593,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="A32" s="10" t="s">
         <v>145</v>
       </c>
@@ -4530,7 +4620,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13">
       <c r="A33" s="10" t="s">
         <v>146</v>
       </c>
@@ -4557,7 +4647,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13">
       <c r="A34" s="10" t="s">
         <v>147</v>
       </c>
@@ -4584,7 +4674,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="25.5" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>158</v>
       </c>
@@ -4636,7 +4726,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="19.4140625" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
@@ -4644,7 +4734,7 @@
     <col min="4" max="4" width="138.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="27" t="s">
         <v>40</v>
       </c>
@@ -4658,7 +4748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="66" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>43</v>
       </c>
@@ -4670,7 +4760,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="66" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
@@ -4684,7 +4774,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="83" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="83" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>119</v>
       </c>
@@ -4698,7 +4788,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="179" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="179" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>125</v>
       </c>
@@ -4712,91 +4802,91 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="53" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="53" customFormat="1" ht="48" customHeight="1">
       <c r="A6" s="50"/>
       <c r="B6" s="50"/>
       <c r="C6" s="51"/>
       <c r="D6" s="52"/>
     </row>
-    <row r="7" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="43.5" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="7"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="7"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="7"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="7"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="7"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="7"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="7"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="7"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="7"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="7"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="7"/>
@@ -4817,7 +4907,7 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="42.9140625" customWidth="1"/>
     <col min="2" max="2" width="29.9140625" customWidth="1"/>
@@ -4827,7 +4917,7 @@
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="59.5" customHeight="1">
       <c r="A1" s="79" t="s">
         <v>222</v>
       </c>
@@ -4837,15 +4927,15 @@
       <c r="C1" s="79" t="s">
         <v>228</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="92" t="s">
         <v>210</v>
       </c>
-      <c r="E1" s="95"/>
+      <c r="E1" s="93"/>
       <c r="F1" s="80" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="86">
         <v>1</v>
       </c>
@@ -4861,11 +4951,11 @@
       <c r="E2" s="6">
         <v>0</v>
       </c>
-      <c r="F2" s="96" t="s">
+      <c r="F2" s="94" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="86">
         <v>1</v>
       </c>
@@ -4881,9 +4971,9 @@
       <c r="E3" s="6">
         <v>9</v>
       </c>
-      <c r="F3" s="97"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="95"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="86">
         <v>1</v>
       </c>
@@ -4899,11 +4989,11 @@
       <c r="E4" s="82">
         <v>0</v>
       </c>
-      <c r="F4" s="98" t="s">
+      <c r="F4" s="96" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="86">
         <v>1</v>
       </c>
@@ -4919,9 +5009,9 @@
       <c r="E5" s="82">
         <v>9</v>
       </c>
-      <c r="F5" s="99"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="97"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="86">
         <v>1</v>
       </c>
@@ -4937,11 +5027,11 @@
       <c r="E6" s="6">
         <v>0</v>
       </c>
-      <c r="F6" s="92" t="s">
+      <c r="F6" s="90" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="86">
         <v>1</v>
       </c>
@@ -4957,9 +5047,9 @@
       <c r="E7" s="6">
         <v>9</v>
       </c>
-      <c r="F7" s="93"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" s="91"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="86">
         <v>1</v>
       </c>
@@ -4975,11 +5065,11 @@
       <c r="E8" s="82">
         <v>0</v>
       </c>
-      <c r="F8" s="90" t="s">
+      <c r="F8" s="98" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="86">
         <v>1</v>
       </c>
@@ -4995,9 +5085,9 @@
       <c r="E9" s="82">
         <v>9</v>
       </c>
-      <c r="F9" s="91"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" s="99"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="86">
         <v>1</v>
       </c>
@@ -5013,11 +5103,11 @@
       <c r="E10" s="6">
         <v>0</v>
       </c>
-      <c r="F10" s="92" t="s">
+      <c r="F10" s="90" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="86">
         <v>1</v>
       </c>
@@ -5033,9 +5123,9 @@
       <c r="E11" s="6">
         <v>9</v>
       </c>
-      <c r="F11" s="93"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" s="91"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="86">
         <v>1</v>
       </c>
@@ -5047,11 +5137,11 @@
       </c>
       <c r="D12" s="82"/>
       <c r="E12" s="82"/>
-      <c r="F12" s="91" t="s">
+      <c r="F12" s="99" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" s="86">
         <v>1</v>
       </c>
@@ -5063,9 +5153,9 @@
       </c>
       <c r="D13" s="82"/>
       <c r="E13" s="82"/>
-      <c r="F13" s="91"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" s="99"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="86">
         <v>1</v>
       </c>
@@ -5081,11 +5171,11 @@
       <c r="E14" s="6">
         <v>0</v>
       </c>
-      <c r="F14" s="92" t="s">
+      <c r="F14" s="90" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="86">
         <v>1</v>
       </c>
@@ -5101,9 +5191,9 @@
       <c r="E15" s="6">
         <v>9</v>
       </c>
-      <c r="F15" s="93"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="91"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="86">
         <v>1</v>
       </c>
@@ -5119,11 +5209,11 @@
       <c r="E16" s="82">
         <v>0</v>
       </c>
-      <c r="F16" s="90" t="s">
+      <c r="F16" s="98" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" s="86">
         <v>1</v>
       </c>
@@ -5139,9 +5229,9 @@
       <c r="E17" s="82">
         <v>9</v>
       </c>
-      <c r="F17" s="91"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="99"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="86">
         <v>1</v>
       </c>
@@ -5157,11 +5247,11 @@
       <c r="E18" s="6">
         <v>0</v>
       </c>
-      <c r="F18" s="92" t="s">
+      <c r="F18" s="90" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" s="86">
         <v>1</v>
       </c>
@@ -5177,9 +5267,9 @@
       <c r="E19" s="6">
         <v>9</v>
       </c>
-      <c r="F19" s="93"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="91"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="86">
         <v>1</v>
       </c>
@@ -5195,11 +5285,11 @@
       <c r="E20" s="82">
         <v>0</v>
       </c>
-      <c r="F20" s="90" t="s">
+      <c r="F20" s="98" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="86">
         <v>1</v>
       </c>
@@ -5215,9 +5305,9 @@
       <c r="E21" s="82">
         <v>9</v>
       </c>
-      <c r="F21" s="91"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F21" s="99"/>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="86">
         <v>1</v>
       </c>
@@ -5233,11 +5323,11 @@
       <c r="E22" s="6">
         <v>0</v>
       </c>
-      <c r="F22" s="92" t="s">
+      <c r="F22" s="90" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" s="86">
         <v>1</v>
       </c>
@@ -5253,9 +5343,9 @@
       <c r="E23" s="6">
         <v>9</v>
       </c>
-      <c r="F23" s="93"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F23" s="91"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="86">
         <v>1</v>
       </c>
@@ -5271,11 +5361,11 @@
       <c r="E24" s="82">
         <v>0</v>
       </c>
-      <c r="F24" s="90" t="s">
+      <c r="F24" s="98" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" s="86">
         <v>1</v>
       </c>
@@ -5291,9 +5381,9 @@
       <c r="E25" s="82">
         <v>9</v>
       </c>
-      <c r="F25" s="91"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F25" s="99"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="86">
         <v>1</v>
       </c>
@@ -5309,11 +5399,11 @@
       <c r="E26" s="6">
         <v>0</v>
       </c>
-      <c r="F26" s="92" t="s">
+      <c r="F26" s="90" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" s="86">
         <v>1</v>
       </c>
@@ -5329,9 +5419,9 @@
       <c r="E27" s="6">
         <v>9</v>
       </c>
-      <c r="F27" s="93"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F27" s="91"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="86">
         <v>1</v>
       </c>
@@ -5347,11 +5437,11 @@
       <c r="E28" s="82">
         <v>0</v>
       </c>
-      <c r="F28" s="90" t="s">
+      <c r="F28" s="98" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" s="86">
         <v>1</v>
       </c>
@@ -5367,9 +5457,9 @@
       <c r="E29" s="82">
         <v>9</v>
       </c>
-      <c r="F29" s="91"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F29" s="99"/>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="86">
         <v>1</v>
       </c>
@@ -5385,11 +5475,11 @@
       <c r="E30" s="6">
         <v>0</v>
       </c>
-      <c r="F30" s="92" t="s">
+      <c r="F30" s="90" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31" s="86">
         <v>1</v>
       </c>
@@ -5405,27 +5495,27 @@
       <c r="E31" s="6">
         <v>9</v>
       </c>
-      <c r="F31" s="93"/>
-    </row>
-    <row r="46" spans="1:2" ht="84.5" x14ac:dyDescent="0.3">
+      <c r="F31" s="91"/>
+    </row>
+    <row r="46" spans="1:2" ht="84.5">
       <c r="A46" s="87" t="s">
         <v>231</v>
       </c>
       <c r="B46" s="88"/>
     </row>
-    <row r="47" spans="1:2" ht="74" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="74">
       <c r="A47" s="89" t="s">
         <v>159</v>
       </c>
       <c r="B47" s="88"/>
     </row>
-    <row r="48" spans="1:2" ht="95" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="95">
       <c r="A48" s="89" t="s">
         <v>232</v>
       </c>
       <c r="B48" s="88"/>
     </row>
-    <row r="49" spans="1:2" ht="147.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="147.5">
       <c r="A49" s="89" t="s">
         <v>168</v>
       </c>
@@ -5435,12 +5525,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="F28:F29"/>
@@ -5451,6 +5535,12 @@
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>